<commit_message>
essas mudanças devem ser o suficiente pra evitar problemas com o limite da API
</commit_message>
<xml_diff>
--- a/data/processed/infl_base.xlsx
+++ b/data/processed/infl_base.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t>screen_name</t>
   </si>
@@ -64,20 +64,16 @@
     <t>politica</t>
   </si>
   <si>
-    <t xml:space="preserve">ShitpostBot 5000
-</t>
-  </si>
-  <si>
-    <t>VERDADEIRO</t>
-  </si>
-  <si>
-    <t>Surreal Memes Bot</t>
+    <t>ShitpostBot5000</t>
+  </si>
+  <si>
+    <t>MemesSurreal</t>
   </si>
   <si>
     <t>905505009667846144</t>
   </si>
   <si>
-    <t>Nath Finanças</t>
+    <t>nathfinancas</t>
   </si>
   <si>
     <t>916008599205359617</t>
@@ -89,43 +85,205 @@
     <t>esquerda</t>
   </si>
   <si>
-    <t>FALSO</t>
-  </si>
-  <si>
-    <t>Rodrigo Vizeu</t>
+    <t>rodrigovizeu</t>
   </si>
   <si>
     <t>jornalista</t>
   </si>
   <si>
-    <t xml:space="preserve">politica
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSO
-</t>
-  </si>
-  <si>
-    <t>Bruno Sartori</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jornalista
-</t>
+    <t>brunnosarttori</t>
+  </si>
+  <si>
+    <t>wesbos</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>ciencia</t>
+  </si>
+  <si>
+    <t>marcelodedois</t>
+  </si>
+  <si>
+    <t>musica</t>
+  </si>
+  <si>
+    <t>AOC</t>
+  </si>
+  <si>
+    <t>G0ffThew</t>
+  </si>
+  <si>
+    <t>anime</t>
+  </si>
+  <si>
+    <t>geek</t>
+  </si>
+  <si>
+    <t>legadaodamassa</t>
+  </si>
+  <si>
+    <t>futebol</t>
+  </si>
+  <si>
+    <t>kmendoncafilho</t>
+  </si>
+  <si>
+    <t>audiovisual</t>
+  </si>
+  <si>
+    <t>arte</t>
+  </si>
+  <si>
+    <t>ObsNaturalistas</t>
+  </si>
+  <si>
+    <t>mineposting1999</t>
+  </si>
+  <si>
+    <t>1161707821106442241</t>
+  </si>
+  <si>
+    <t>benozzatiarthur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">humor </t>
+  </si>
+  <si>
+    <t>lgbtq</t>
+  </si>
+  <si>
+    <t>marcelorubens</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>palmeiras</t>
+  </si>
+  <si>
+    <t>flamengo</t>
+  </si>
+  <si>
+    <t>gremio</t>
+  </si>
+  <si>
+    <t>cruzeiro</t>
+  </si>
+  <si>
+    <t>santosFC</t>
+  </si>
+  <si>
+    <t>AthleticoPR</t>
+  </si>
+  <si>
+    <t>Atletico</t>
+  </si>
+  <si>
+    <t>Corinthians</t>
+  </si>
+  <si>
+    <t>EmojiMashupPlus</t>
+  </si>
+  <si>
+    <t>1175292276769198080</t>
+  </si>
+  <si>
+    <t>EmojiMashupBot</t>
+  </si>
+  <si>
+    <t>1150993041513177088</t>
+  </si>
+  <si>
+    <t>congresseditors</t>
+  </si>
+  <si>
+    <t>AcidInfusionMil</t>
+  </si>
+  <si>
+    <t>900369802988056577</t>
+  </si>
+  <si>
+    <t>_IloveAnimais_</t>
+  </si>
+  <si>
+    <t>1061258280142553089</t>
+  </si>
+  <si>
+    <t>itimaliasof</t>
+  </si>
+  <si>
+    <t>1061028349752107009</t>
+  </si>
+  <si>
+    <t>QuebrandoOTabu</t>
+  </si>
+  <si>
+    <t>whindersson</t>
+  </si>
+  <si>
+    <t>gatinhogifs</t>
+  </si>
+  <si>
+    <t>1051837863451652097</t>
+  </si>
+  <si>
+    <t>progrbr</t>
+  </si>
+  <si>
+    <t>905539618715688960</t>
+  </si>
+  <si>
+    <t>RealSexyCyborg</t>
+  </si>
+  <si>
+    <t>monark</t>
+  </si>
+  <si>
+    <t>louieponto</t>
+  </si>
+  <si>
+    <t>iMandyCandy</t>
+  </si>
+  <si>
+    <t>LubaTV</t>
+  </si>
+  <si>
+    <t>pabllovittar</t>
+  </si>
+  <si>
+    <t>maisa</t>
+  </si>
+  <si>
+    <t>quadroembranco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font/>
     <font>
+      <sz val="10.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="System-ui"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -143,21 +301,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,7 +542,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.14"/>
+    <col customWidth="1" min="1" max="1" width="16.0"/>
     <col customWidth="1" min="2" max="2" width="20.71"/>
   </cols>
   <sheetData>
@@ -392,7 +559,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -400,64 +567,64 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="b">
+      <c r="E2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="b">
+      <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="b">
+      <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1" t="b">
@@ -465,88 +632,700 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4.462881555E9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="B9" s="1">
+        <v>1.5024328E7</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2">
-        <v>1.5024328E7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>6.4773188E7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1">
+        <v>815246.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.8473551E7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.38203134E8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.12990863E8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.875236456E9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.0308116E7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7.7903908E7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3.0248877E7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.0117765E7</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4.6104914E7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.9591856E7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2.0237983E7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.562061097E9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4.9751816E7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1">
+        <v>9.7208991E7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1">
+        <v>9.0676816E7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4.4627459E7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2.653987092E9</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2.83230411E8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2.30186518E8</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.562121415E9</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2.4296772E8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5.0129112E7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2.409117824E9</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.21517065E8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.74226791E8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2.203709322E9</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2.979201268E9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>